<commit_message>
added cookies presence kpi updated base measure tiers to match set count of kpi
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
+++ b/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
@@ -5,22 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Top-Middle-Bottom" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Count of" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Blocking" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Base Measure" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Product Orientation" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Presence" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Count of Shelves" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Percent" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Aggregation" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Top-Middle-Bottom Map" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Result" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Presence within Bay" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Set Count of" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Blocking" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Base Measure" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Product Orientation" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Presence" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Count of Shelves" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Percent" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Aggregation" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Top-Middle-Bottom Map" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Result" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Presence within Bay" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="121">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -112,12 +113,27 @@
     <t xml:space="preserve">How many items are carried? (4 foot set)</t>
   </si>
   <si>
+    <t xml:space="preserve">Set Count of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many base feet is RBG?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less than or Equal to 2 Feet, 2 Feet &gt; and &lt;= 4 Feet</t>
+  </si>
+  <si>
     <t xml:space="preserve">How many items are carried? (8 foot set)</t>
   </si>
   <si>
+    <t xml:space="preserve">4 Feet &gt; and &lt;= 6 Feet, 6 Feet &gt; and &lt;= 8 Feet</t>
+  </si>
+  <si>
     <t xml:space="preserve">How many items are carried? (12 foot set)</t>
   </si>
   <si>
+    <t xml:space="preserve">8 Feet &gt; and &lt;= 10 Feet, 10 Feet &gt; and &lt;= 12 Feet, Greater than 12 Feet</t>
+  </si>
+  <si>
     <t xml:space="preserve">How many items have more than one facing? (4 foot set)</t>
   </si>
   <si>
@@ -157,9 +173,6 @@
     <t xml:space="preserve">How are Savory segments blocked?</t>
   </si>
   <si>
-    <t xml:space="preserve">How many base feet is RBG?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Base Measure</t>
   </si>
   <si>
@@ -235,6 +248,9 @@
     <t xml:space="preserve">count of</t>
   </si>
   <si>
+    <t xml:space="preserve">Min</t>
+  </si>
+  <si>
     <t xml:space="preserve">GMI_CATEGORY</t>
   </si>
   <si>
@@ -244,6 +260,9 @@
     <t xml:space="preserve">product_ean_code</t>
   </si>
   <si>
+    <t xml:space="preserve">quartile</t>
+  </si>
+  <si>
     <t xml:space="preserve">blocking</t>
   </si>
   <si>
@@ -316,9 +335,6 @@
     <t xml:space="preserve">TTL R CKY CHOCOLATE CHIP</t>
   </si>
   <si>
-    <t xml:space="preserve">quartile</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOS Type</t>
   </si>
   <si>
@@ -370,7 +386,7 @@
     <t xml:space="preserve">Vertical Block, Horizontal Block, Not Blocked</t>
   </si>
   <si>
-    <t xml:space="preserve">Less than or Equal to 2 Feet, 2 Feet &gt; and &lt;= 4 Feet, 4 Feet &gt; and &lt;= 6 Feet, 6 Feet &gt; and &lt;= 8 Feet, Greater than 8 Feet</t>
+    <t xml:space="preserve">Less than or Equal to 2 Feet, 2 Feet &gt; and &lt;= 4 Feet, 4 Feet &gt; and &lt;= 6 Feet, 6 Feet &gt; and &lt;= 8 Feet, 8 Feet &gt; and &lt;= 10 Feet, 10 Feet &gt; and &lt;= 12 Feet, Greater than 12 Feet</t>
   </si>
   <si>
     <t xml:space="preserve">Yes, No</t>
@@ -591,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -600,7 +616,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.0333333333333"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7185185185185"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.05555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.237037037037"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8555555555556"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="106.225925925926"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3888888888889"/>
@@ -852,13 +868,17 @@
         <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F13" s="0" t="s">
         <v>12</v>
       </c>
@@ -868,16 +888,20 @@
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F14" s="0" t="s">
         <v>12</v>
       </c>
@@ -887,16 +911,20 @@
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F15" s="0" t="s">
         <v>12</v>
       </c>
@@ -904,18 +932,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
       <c r="F16" s="0" t="s">
         <v>12</v>
       </c>
@@ -923,18 +955,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F17" s="0" t="s">
         <v>12</v>
       </c>
@@ -942,18 +978,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F18" s="0" t="s">
         <v>12</v>
       </c>
@@ -963,10 +1003,10 @@
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>11</v>
@@ -982,10 +1022,10 @@
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>11</v>
@@ -1001,10 +1041,10 @@
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>11</v>
@@ -1020,10 +1060,10 @@
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>11</v>
@@ -1039,10 +1079,10 @@
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>11</v>
@@ -1058,10 +1098,10 @@
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>11</v>
@@ -1077,10 +1117,10 @@
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>11</v>
@@ -1096,10 +1136,10 @@
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>11</v>
@@ -1115,10 +1155,10 @@
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
@@ -1134,10 +1174,10 @@
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>11</v>
@@ -1153,10 +1193,10 @@
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>11</v>
@@ -1172,10 +1212,10 @@
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>11</v>
@@ -1191,10 +1231,10 @@
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>11</v>
@@ -1210,10 +1250,10 @@
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>11</v>
@@ -1238,6 +1278,79 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.8814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.84074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1262,24 +1375,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1293,7 +1406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1311,7 +1424,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B1" s="5" t="n">
         <v>1</v>
@@ -1349,13 +1462,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1370,16 +1483,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1393,19 +1506,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -1418,22 +1531,22 @@
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -1445,25 +1558,25 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1474,28 +1587,28 @@
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1505,210 +1618,67 @@
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="104.851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.07407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="0" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1727,9 +1697,152 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="104.851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.07407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1744,15 +1857,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1791,13 +1904,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,13 +1918,13 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,13 +1932,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,13 +1946,13 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,13 +1960,13 @@
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,13 +1974,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1875,13 +1988,13 @@
         <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1900,15 +2013,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.0333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.4037037037037"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6407407407407"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3592592592593"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6407407407407"/>
@@ -1921,16 +2034,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,16 +2051,16 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1955,16 +2068,16 @@
         <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,16 +2085,16 @@
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,16 +2102,16 @@
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,102 +2119,24 @@
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2114,6 +2149,177 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.3444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2138,111 +2344,111 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2256,7 +2462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2281,27 +2487,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2315,7 +2521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2345,57 +2551,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2409,7 +2615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2435,35 +2641,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2477,7 +2683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2502,27 +2708,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2534,77 +2740,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.8814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added presence kpi finished orient kpi added irrelevant products back into certain kpis added set_count of kpi RBG ready for testing
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
+++ b/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="127">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">GMI</t>
   </si>
   <si>
-    <t xml:space="preserve">Main Stocking Location for Refrigerated Baked Goods, Separate Natural</t>
+    <t xml:space="preserve">Main Stocking Location for Refrigerated Baked Goods</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
@@ -296,6 +296,9 @@
     <t xml:space="preserve">CAN</t>
   </si>
   <si>
+    <t xml:space="preserve">orient</t>
+  </si>
+  <si>
     <t xml:space="preserve">param 1</t>
   </si>
   <si>
@@ -396,6 +399,21 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;5, 5, 6, 7, 8+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 FT SET - ALL Cans stocked on end, 4 FT SET - ALL Cans stocked on side, 4 FT SET - Mix of orientation, 6 FT SET - ALL Cans stocked on end, 6 FT SET - ALL Cans stocked on side, 6 FT SET - Mix of orientation, 8 FT SET - ALL Cans stocked on end, 8 FT SET - ALL Cans stocked on side, 8 FT SET - Mix of orientation, 10 FT SET - ALL Cans stocked on end, 10 FT SET - ALL Cans stocked on side, 10 FT SET - Mix of orientation, 12 FT SET - ALL Cans stocked on end, 12 FT SET - ALL Cans stocked on side, 12 FT SET - Mix of orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pres_bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;5, 5-10%, 10-20%, &gt;=20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excluded param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excluded value 1</t>
   </si>
 </sst>
 </file>
@@ -607,22 +625,22 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="111.714814814815"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.7962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="120.533333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,7 +1200,9 @@
       <c r="C28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="0" t="s">
         <v>12</v>
@@ -1282,21 +1302,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.2333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.362962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.8592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.32962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1304,41 +1324,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1363,11 +1384,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.34814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,10 +1396,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>58</v>
@@ -1389,10 +1410,10 @@
         <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1419,13 +1440,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="5" t="n">
         <v>1</v>
@@ -1463,13 +1484,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1484,16 +1505,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1507,19 +1528,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -1532,22 +1553,22 @@
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -1559,25 +1580,25 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1588,28 +1609,28 @@
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1619,67 +1640,67 @@
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="K9" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1698,33 +1719,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="110.244444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.27037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="118.866666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.76296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,10 +1753,10 @@
         <v>61</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>13</v>
@@ -1746,10 +1767,10 @@
         <v>69</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>114</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>13</v>
@@ -1760,10 +1781,10 @@
         <v>75</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>13</v>
@@ -1774,10 +1795,10 @@
         <v>78</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>13</v>
@@ -1785,13 +1806,13 @@
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>13</v>
@@ -1799,13 +1820,13 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>13</v>
@@ -1813,15 +1834,43 @@
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1841,32 +1890,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.9222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1893,11 +1956,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.9555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.8777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.03703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2022,12 +2085,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.4222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.3222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2150,19 +2213,19 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.7592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.0222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2332,11 +2395,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,11 +2538,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,24 +2589,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.03703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2574,6 +2637,9 @@
       <c r="I1" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -2602,6 +2668,9 @@
       </c>
       <c r="I2" s="0" t="s">
         <v>63</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2628,12 +2697,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="109.262962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="117.885185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2641,10 +2710,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>58</v>
@@ -2661,15 +2730,15 @@
         <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2696,11 +2765,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2728,7 +2797,7 @@
         <v>72</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
variety of changes to bring results inline with expected results
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
+++ b/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="127">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -260,6 +260,9 @@
     <t xml:space="preserve">product_fk</t>
   </si>
   <si>
+    <t xml:space="preserve">quartile</t>
+  </si>
+  <si>
     <t xml:space="preserve">blocking</t>
   </si>
   <si>
@@ -333,9 +336,6 @@
   </si>
   <si>
     <t xml:space="preserve">TTL R CKY CHOCOLATE CHIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quartile</t>
   </si>
   <si>
     <t xml:space="preserve">SOS Type</t>
@@ -626,21 +626,21 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.7962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="120.533333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.52592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.8333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.84074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="126.803703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,13 +1310,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.8592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.4074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.9111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,16 +1324,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>58</v>
@@ -1344,10 +1344,10 @@
         <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>59</v>
@@ -1356,7 +1356,7 @@
         <v>60</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1384,11 +1384,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.54444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,19 +1432,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>105</v>
       </c>
@@ -1703,6 +1703,8 @@
         <v>108</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1727,11 +1729,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="118.866666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.76296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="125.040740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.15185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,7 +1780,7 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>117</v>
@@ -1792,7 +1794,7 @@
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>118</v>
@@ -1806,7 +1808,7 @@
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>119</v>
@@ -1820,7 +1822,7 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>120</v>
@@ -1834,7 +1836,7 @@
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>121</v>
@@ -1848,7 +1850,7 @@
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>122</v>
@@ -1892,16 +1894,16 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.9222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.0777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,11 +1958,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.8777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.6222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2085,12 +2087,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.3222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.7518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.062962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,18 +2216,18 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.0222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.4259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2330,6 +2332,9 @@
       <c r="F5" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="G5" s="0" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -2350,6 +2355,9 @@
       <c r="F6" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="G6" s="0" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -2369,6 +2377,9 @@
       </c>
       <c r="F7" s="0" t="s">
         <v>74</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2395,11 +2406,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.1185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,7 +2438,7 @@
         <v>62</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,7 +2452,7 @@
         <v>60</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,7 +2466,7 @@
         <v>66</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,7 +2480,7 @@
         <v>65</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2483,7 +2494,7 @@
         <v>63</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,10 +2505,10 @@
         <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2508,10 +2519,10 @@
         <v>59</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2538,11 +2549,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.062962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2570,7 +2581,7 @@
         <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2597,16 +2608,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,22 +2631,22 @@
         <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>58</v>
@@ -2646,10 +2657,10 @@
         <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>59</v>
@@ -2670,7 +2681,7 @@
         <v>63</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2697,12 +2708,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="117.885185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.4703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="123.962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2710,10 +2721,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>58</v>
@@ -2730,15 +2741,15 @@
         <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2765,11 +2776,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,7 +2808,7 @@
         <v>72</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated topmiddlebottom partially updated count of shelves
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
+++ b/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="128">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t xml:space="preserve">*Still waiting on confirmation of attributes to be used for this KPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Threshold</t>
   </si>
   <si>
     <t xml:space="preserve">count of shelves</t>
@@ -626,21 +629,21 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="E4:E5 D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.8333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="126.803703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.4037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.93703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="130.037037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,18 +1308,18 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="E4:E5 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.4074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.9111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.52592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.5148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,16 +1327,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>58</v>
@@ -1344,10 +1347,10 @@
         <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>59</v>
@@ -1379,16 +1382,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="E4:E5 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.54444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.0037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,10 +1399,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>58</v>
@@ -1410,10 +1413,10 @@
         <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1434,19 +1437,19 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="E4:E5 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="5" t="n">
         <v>1</v>
@@ -1484,13 +1487,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1505,16 +1508,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1528,19 +1531,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -1553,22 +1556,22 @@
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -1580,25 +1583,25 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1609,28 +1612,28 @@
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1640,67 +1643,67 @@
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="K9" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1724,30 +1727,30 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="E4:E5 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="125.040740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.15185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="128.177777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.25185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,10 +1758,10 @@
         <v>61</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>13</v>
@@ -1769,10 +1772,10 @@
         <v>69</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>115</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>13</v>
@@ -1783,10 +1786,10 @@
         <v>76</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>13</v>
@@ -1797,10 +1800,10 @@
         <v>79</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>13</v>
@@ -1811,10 +1814,10 @@
         <v>91</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>13</v>
@@ -1825,10 +1828,10 @@
         <v>75</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>13</v>
@@ -1836,13 +1839,13 @@
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>13</v>
@@ -1853,10 +1856,10 @@
         <v>88</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>13</v>
@@ -1864,13 +1867,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>13</v>
@@ -1895,15 +1898,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="E4:E5 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.0777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.2518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.0222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,10 +1914,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>58</v>
@@ -1931,7 +1934,7 @@
         <v>72</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1953,16 +1956,16 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="E4:E5 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.6222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.0888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.32962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2082,17 +2085,17 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="E4:E5 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.7518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.062962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.5148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,18 +2219,18 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="E4:E5 C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.4259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.7962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.4740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2401,16 +2404,16 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="1" sqref="E4:E5 F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.1185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2544,16 +2547,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="E4:E5 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.062962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,21 +2606,21 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="E4:E5 B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.32962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2703,17 +2706,17 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="E4:E5 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.4703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="123.962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="127.196296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2768,22 +2771,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2794,10 +2797,13 @@
         <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>51</v>
       </c>
@@ -2807,8 +2813,11 @@
       <c r="C2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>94</v>
+      <c r="D2" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated shelf count rbg only hack
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
+++ b/Projects/GMIUS/Data/RBG GMI KPI Template v0.5.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="127">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -315,9 +315,6 @@
   </si>
   <si>
     <t xml:space="preserve">*Still waiting on confirmation of attributes to be used for this KPI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Threshold</t>
   </si>
   <si>
     <t xml:space="preserve">count of shelves</t>
@@ -629,21 +626,21 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="E4:E5 D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.4037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.93703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="130.037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.9703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.03703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="133.37037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1308,18 +1305,18 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="E4:E5 C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.7777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.5148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,16 +1324,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>58</v>
@@ -1347,10 +1344,10 @@
         <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>59</v>
@@ -1382,16 +1379,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="E4:E5 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.0037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,10 +1396,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>58</v>
@@ -1413,10 +1410,10 @@
         <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1438,18 +1435,18 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="E4:E5 B10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="5" t="n">
         <v>1</v>
@@ -1487,13 +1484,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1508,16 +1505,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1531,19 +1528,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -1556,22 +1553,22 @@
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -1583,25 +1580,25 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="F6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1612,28 +1609,28 @@
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="F7" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1643,67 +1640,67 @@
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="F8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="F9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1727,30 +1724,30 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="E4:E5 B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="128.177777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.25185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="131.507407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.34814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,10 +1755,10 @@
         <v>61</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>116</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>13</v>
@@ -1772,10 +1769,10 @@
         <v>69</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>13</v>
@@ -1786,10 +1783,10 @@
         <v>76</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>13</v>
@@ -1800,10 +1797,10 @@
         <v>79</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>13</v>
@@ -1814,10 +1811,10 @@
         <v>91</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>13</v>
@@ -1828,10 +1825,10 @@
         <v>75</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>13</v>
@@ -1839,13 +1836,13 @@
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>13</v>
@@ -1856,10 +1853,10 @@
         <v>88</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>13</v>
@@ -1867,13 +1864,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>125</v>
-      </c>
       <c r="C10" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>13</v>
@@ -1898,15 +1895,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="E4:E5 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.2518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.0222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.3296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,10 +1911,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>127</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>58</v>
@@ -1934,7 +1931,7 @@
         <v>72</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1956,16 +1953,16 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="E4:E5 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.0888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.5592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.42592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2085,17 +2082,17 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="E4:E5 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.5148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.3777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2219,18 +2216,18 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="E4:E5 C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.7962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.4740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.2666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2404,16 +2401,16 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="1" sqref="E4:E5 F14"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,16 +2544,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="E4:E5 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,21 +2603,21 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="E4:E5 B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.42592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2706,17 +2703,17 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="E4:E5 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="127.196296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="130.42962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2771,19 +2768,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E4:E5"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,9 +2794,6 @@
         <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="0" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2813,11 +2807,8 @@
       <c r="C2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>95</v>
+      <c r="D2" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>